<commit_message>
Se actalizaron algunos archivos
Se actalizaron algunos archivos
</commit_message>
<xml_diff>
--- a/Proyecto1/Normex Modulos.xlsx
+++ b/Proyecto1/Normex Modulos.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SKYLINE\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositorio\Normex\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="8340" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="61">
   <si>
     <t xml:space="preserve">1.- </t>
   </si>
@@ -202,34 +202,13 @@
     <t>M</t>
   </si>
   <si>
-    <t>Carga de huertos sorteados por APEAM (entrega semanal)</t>
-  </si>
-  <si>
-    <t>Impresión de etiquetas con folio de recepcion.</t>
-  </si>
-  <si>
-    <t>Verificar parametros de envio y maximos, consumir N veces WebService (por cada rechazo) y actualizar estatus de estudio en BD. Construir XTML llenarlo con la BD (estudios realizados) y actualizar estatus de correos enviados.</t>
-  </si>
-  <si>
-    <t>7.-</t>
-  </si>
-  <si>
-    <t>Consumo de WebService</t>
-  </si>
-  <si>
-    <t>Cargar al Storage, registrar en BD nube, construir interfaz txt para  consumir WebService y registrar codigo respuesta. Buscar dentro del excel, celdas de analistos, SAGARPA y  nombre del productor, validar.</t>
-  </si>
-  <si>
-    <t>Pasar a BD APEAM resultado de analitos</t>
-  </si>
-  <si>
-    <t>Constos mensuales</t>
-  </si>
-  <si>
-    <t>Computo en nube Microsoft</t>
-  </si>
-  <si>
-    <t>Conexión VPN segura</t>
+    <t>Decodificación de resultado de análsis</t>
+  </si>
+  <si>
+    <t>Gestor de envíos de listado de resultados</t>
+  </si>
+  <si>
+    <t>Seguridad y parametrización de aplicaciones</t>
   </si>
 </sst>
 </file>
@@ -588,10 +567,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -642,7 +621,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>58</v>
+        <v>4</v>
       </c>
       <c r="D5">
         <v>14</v>
@@ -655,16 +634,13 @@
       <c r="D6">
         <v>16</v>
       </c>
-      <c r="F6" t="s">
-        <v>59</v>
-      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>22</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -707,7 +683,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>24</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -750,7 +726,7 @@
         <v>24</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>60</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -793,7 +769,7 @@
         <v>33</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -845,14 +821,6 @@
       </c>
       <c r="D29">
         <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>61</v>
-      </c>
-      <c r="B30" t="s">
-        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -863,10 +831,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H39"/>
+  <dimension ref="B1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+    <sheetView topLeftCell="A15" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -875,7 +843,7 @@
     <col min="2" max="2" width="37.5703125" customWidth="1"/>
     <col min="3" max="3" width="6.140625" customWidth="1"/>
     <col min="4" max="4" width="38.85546875" customWidth="1"/>
-    <col min="8" max="8" width="79.7109375" customWidth="1"/>
+    <col min="8" max="8" width="79.7109375" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" x14ac:dyDescent="0.25">
@@ -886,11 +854,11 @@
         <v>1</v>
       </c>
       <c r="E1">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F1">
         <f>E1/10</f>
-        <v>1</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
@@ -901,11 +869,11 @@
         <v>2</v>
       </c>
       <c r="E2">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F2">
-        <f t="shared" ref="F2:F23" si="0">E2/10</f>
-        <v>1</v>
+        <f t="shared" ref="F2:F22" si="0">E2/10</f>
+        <v>1.2</v>
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
@@ -916,11 +884,11 @@
         <v>3</v>
       </c>
       <c r="E3">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
@@ -998,7 +966,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="9" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>22</v>
       </c>
@@ -1006,38 +974,37 @@
         <v>9</v>
       </c>
       <c r="E9">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="F9">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>3.2</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>63</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>62</v>
+        <v>24</v>
       </c>
       <c r="D10" t="s">
-        <v>64</v>
+        <v>11</v>
       </c>
       <c r="E10">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="F10">
         <f t="shared" si="0"/>
-        <v>2.4</v>
-      </c>
-      <c r="H10" s="2"/>
+        <v>0.8</v>
+      </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E11">
         <v>8</v>
@@ -1052,7 +1019,7 @@
         <v>24</v>
       </c>
       <c r="D12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E12">
         <v>8</v>
@@ -1062,37 +1029,37 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" t="s">
+        <v>35</v>
+      </c>
+      <c r="E13">
         <v>24</v>
       </c>
-      <c r="D13" t="s">
-        <v>13</v>
-      </c>
-      <c r="E13">
-        <v>8</v>
-      </c>
       <c r="F13">
         <f t="shared" si="0"/>
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+        <v>2.4</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="D14" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E14">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="F14">
         <f t="shared" si="0"/>
-        <v>3.2</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>60</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
@@ -1100,14 +1067,17 @@
         <v>25</v>
       </c>
       <c r="D15" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E15">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="F15">
         <f t="shared" si="0"/>
-        <v>0.4</v>
+        <v>1.2</v>
+      </c>
+      <c r="H15" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
@@ -1115,32 +1085,29 @@
         <v>25</v>
       </c>
       <c r="D16" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="E16">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F16">
         <f t="shared" si="0"/>
-        <v>1.2</v>
-      </c>
-      <c r="H16" t="s">
-        <v>39</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="D17" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E17">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F17">
         <f t="shared" si="0"/>
-        <v>1.2</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
@@ -1148,14 +1115,14 @@
         <v>16</v>
       </c>
       <c r="D18" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E18">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F18">
         <f t="shared" si="0"/>
-        <v>1.2</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
@@ -1163,14 +1130,14 @@
         <v>16</v>
       </c>
       <c r="D19" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="E19">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F19">
         <f t="shared" si="0"/>
-        <v>1.2</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
@@ -1178,22 +1145,22 @@
         <v>16</v>
       </c>
       <c r="D20" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E20">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="F20">
         <f t="shared" si="0"/>
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D21" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E21">
         <v>4</v>
@@ -1202,38 +1169,38 @@
         <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
-    </row>
-    <row r="22" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H21" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D22" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="E22">
         <v>4</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="3">
         <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
-      <c r="H22" s="2" t="s">
-        <v>30</v>
-      </c>
+      <c r="G22" s="3"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="D23" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
       <c r="E23">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F23" s="3">
-        <f t="shared" si="0"/>
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="G23" s="3"/>
     </row>
@@ -1242,13 +1209,13 @@
         <v>40</v>
       </c>
       <c r="D24" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="E24">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="F24" s="3">
-        <v>0.6</v>
+        <v>0</v>
       </c>
       <c r="G24" s="3"/>
     </row>
@@ -1257,13 +1224,13 @@
         <v>40</v>
       </c>
       <c r="D25" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E25">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F25" s="3">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="G25" s="3"/>
     </row>
@@ -1272,28 +1239,28 @@
         <v>40</v>
       </c>
       <c r="D26" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E26">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F26" s="3">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="G26" s="3"/>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="D27" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="E27">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="F27" s="3">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="G27" s="3"/>
     </row>
@@ -1302,104 +1269,57 @@
         <v>45</v>
       </c>
       <c r="D28" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E28">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="F28" s="3">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="G28" s="3"/>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D29" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E29">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="F29" s="3">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="G29" s="3"/>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B30" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D30" t="s">
-        <v>49</v>
-      </c>
       <c r="E30">
-        <v>16</v>
-      </c>
-      <c r="F30" s="3">
-        <v>1.6</v>
-      </c>
-      <c r="G30" s="3"/>
+        <f>SUM(E1:E29)</f>
+        <v>274</v>
+      </c>
+      <c r="F30">
+        <f>SUM(F1:F29)</f>
+        <v>24.199999999999996</v>
+      </c>
+      <c r="G30">
+        <f>SUM(E30:F30)</f>
+        <v>298.2</v>
+      </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B31" s="1"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
+      <c r="F31" t="s">
+        <v>50</v>
+      </c>
+      <c r="G31" s="4">
+        <v>300</v>
+      </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="E32">
-        <f>SUM(E1:E30)</f>
-        <v>341</v>
-      </c>
-      <c r="F32">
-        <f>SUM(F1:F30)</f>
-        <v>32.4</v>
-      </c>
-      <c r="G32">
-        <f>SUM(E32:F32)</f>
-        <v>373.4</v>
-      </c>
-    </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="F33" t="s">
-        <v>50</v>
-      </c>
-      <c r="G33" s="4">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="G34" s="4">
-        <f>G32*G33</f>
-        <v>93350</v>
-      </c>
-    </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
-        <v>66</v>
-      </c>
-      <c r="G37" s="4">
-        <v>2450</v>
-      </c>
-    </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
-        <v>67</v>
-      </c>
-      <c r="G38" s="4">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="G39" s="4">
-        <f>SUM(G37:G38)</f>
-        <v>2670</v>
+      <c r="G32" s="4">
+        <f>G30*G31</f>
+        <v>89460</v>
       </c>
     </row>
   </sheetData>
@@ -1412,7 +1332,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:AH35"/>
   <sheetViews>
-    <sheetView zoomScale="98" zoomScaleNormal="98" workbookViewId="0"/>
+    <sheetView topLeftCell="C1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>